<commit_message>
some new umit added
</commit_message>
<xml_diff>
--- a/umit_files/umit_ang.xlsx
+++ b/umit_files/umit_ang.xlsx
@@ -21,10 +21,12 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,11 +262,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1Uwtd7r9E8nDHAxUMRJfuO86povMpGnWIVX-1Pwd7LIQ/edit?usp=sharing"",""УМИТЫ!A:Z"")"),"Грамматика")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1FqnxW1nvn6x-1AvpP8JTyc3IKWPdjv5B_SLFZCc8kE8/edit"",""УМИТЫ!A:Z"")"),"Грамматика")</f>
         <v>Грамматика</v>
       </c>
       <c r="B1" s="1"/>
@@ -3030,8 +3032,14 @@
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),57.0)</f>
         <v>57</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="C58" s="1" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Вопросительные предложения в Future Perfect Continuous")</f>
+        <v>Вопросительные предложения в Future Perfect Continuous</v>
+      </c>
+      <c r="D58" s="1">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),157.0)</f>
+        <v>157</v>
+      </c>
       <c r="E58" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Лексика ""Досуг и увлечения""")</f>
         <v>Лексика "Досуг и увлечения"</v>
@@ -4072,8 +4080,14 @@
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="E84" s="1" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Relationships and people, Materials and the built environment")</f>
+        <v>Relationships and people, Materials and the built environment</v>
+      </c>
+      <c r="F84" s="1">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),283.0)</f>
+        <v>283</v>
+      </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -4470,8 +4484,14 @@
       <c r="Z95" s="1"/>
     </row>
     <row r="96">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="1" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"For-to construction, Causative form")</f>
+        <v>For-to construction, Causative form</v>
+      </c>
+      <c r="B96" s="1">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),94.0)</f>
+        <v>94</v>
+      </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>

</xml_diff>

<commit_message>
new umits 22 oct
</commit_message>
<xml_diff>
--- a/umit_files/umit_ang.xlsx
+++ b/umit_files/umit_ang.xlsx
@@ -465,8 +465,8 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление артикля a/an")</f>
-        <v>Употребление артикля a/an</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление артикля a")</f>
+        <v>Употребление артикля a</v>
       </c>
       <c r="B4" s="1">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
@@ -1783,12 +1783,12 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Причастия")</f>
-        <v>Причастия</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в простых предложениях")</f>
+        <v>Пунктуация в простых предложениях</v>
       </c>
       <c r="B31" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),30.0)</f>
-        <v>30</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.0)</f>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Past Perfect")</f>
@@ -1829,12 +1829,12 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в простых предложениях")</f>
-        <v>Пунктуация в простых предложениях</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в сложноподчиненных предложениях")</f>
+        <v>Пунктуация в сложноподчиненных предложениях</v>
       </c>
       <c r="B32" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.0)</f>
-        <v>31</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.0)</f>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Past Perfect")</f>
@@ -1875,12 +1875,12 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в сложных предложениях")</f>
-        <v>Пунктуация в сложных предложениях</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Relative Clauses")</f>
+        <v>Relative Clauses</v>
       </c>
       <c r="B33" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
-        <v>32</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Past Perfect")</f>
@@ -1921,12 +1921,12 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в сложноподчиненных предложениях")</f>
-        <v>Пунктуация в сложноподчиненных предложениях</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Согласование времён в косвенной речи")</f>
+        <v>Согласование времён в косвенной речи</v>
       </c>
       <c r="B34" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.0)</f>
-        <v>33</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),35.0)</f>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Future Simple")</f>
@@ -1967,12 +1967,12 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Relative Clauses")</f>
-        <v>Relative Clauses</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательных с помощью -er")</f>
+        <v>Образование сравнительной степени прилагательных с помощью -er</v>
       </c>
       <c r="B35" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
-        <v>34</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),36.0)</f>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Future Simple")</f>
@@ -2013,12 +2013,12 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Согласование времён в косвенной речи")</f>
-        <v>Согласование времён в косвенной речи</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательных с помощью more")</f>
+        <v>Образование сравнительной степени прилагательных с помощью more</v>
       </c>
       <c r="B36" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),35.0)</f>
-        <v>35</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),37.0)</f>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Future Simple")</f>
@@ -2059,12 +2059,12 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательных с помощью -er")</f>
-        <v>Образование сравнительной степени прилагательных с помощью -er</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование превосходной степени прилагательных с помощью -est")</f>
+        <v>Образование превосходной степени прилагательных с помощью -est</v>
       </c>
       <c r="B37" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),36.0)</f>
-        <v>36</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Future Simple")</f>
@@ -2105,12 +2105,12 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательных с помощью more")</f>
-        <v>Образование сравнительной степени прилагательных с помощью more</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Превосходная степень сложных прилагательных")</f>
+        <v>Превосходная степень сложных прилагательных</v>
       </c>
       <c r="B38" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),37.0)</f>
-        <v>37</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),39.0)</f>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Future Continuous")</f>
@@ -2151,12 +2151,12 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование превосходной степени прилагательных с помощью -est")</f>
-        <v>Образование превосходной степени прилагательных с помощью -est</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Исключения в сравнении прилагательных")</f>
+        <v>Исключения в сравнении прилагательных</v>
       </c>
       <c r="B39" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
-        <v>38</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
+        <v>40</v>
       </c>
       <c r="C39" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Who, which, that, whom")</f>
@@ -2197,12 +2197,12 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Превосходная степень сложных прилагательных")</f>
-        <v>Превосходная степень сложных прилагательных</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Оборот as...as")</f>
+        <v>Оборот as...as</v>
       </c>
       <c r="B40" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),39.0)</f>
-        <v>39</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.0)</f>
+        <v>41</v>
       </c>
       <c r="C40" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Предположительные контрукции")</f>
@@ -2243,12 +2243,12 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Исключения в сравнении прилагательных")</f>
-        <v>Исключения в сравнении прилагательных</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инфинитив")</f>
+        <v>Инфинитив</v>
       </c>
       <c r="B41" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
-        <v>40</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),42.0)</f>
+        <v>42</v>
       </c>
       <c r="C41" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Future Continuous")</f>
@@ -2289,12 +2289,12 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Оборот as...as")</f>
-        <v>Оборот as...as</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление Bare Infinitive (инфинитив без частицы to)")</f>
+        <v>Употребление Bare Infinitive (инфинитив без частицы to)</v>
       </c>
       <c r="B42" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.0)</f>
-        <v>41</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43.0)</f>
+        <v>43</v>
       </c>
       <c r="C42" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Future Continuous")</f>
@@ -2335,12 +2335,12 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инфинитив и герундий после глаголов")</f>
-        <v>Инфинитив и герундий после глаголов</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Stative Verbs")</f>
+        <v>Stative Verbs</v>
       </c>
       <c r="B43" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),42.0)</f>
-        <v>42</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
+        <v>44</v>
       </c>
       <c r="C43" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Future Continuous")</f>
@@ -2381,12 +2381,12 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление Bare Infinitive (инфинитив без частицы to)")</f>
-        <v>Употребление Bare Infinitive (инфинитив без частицы to)</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Нулевой тип условных предложений")</f>
+        <v>Нулевой тип условных предложений</v>
       </c>
       <c r="B44" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43.0)</f>
-        <v>43</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45.0)</f>
+        <v>45</v>
       </c>
       <c r="C44" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Future Perfect")</f>
@@ -2427,12 +2427,12 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Stative Verbs")</f>
-        <v>Stative Verbs</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Первый тип условных предложений")</f>
+        <v>Первый тип условных предложений</v>
       </c>
       <c r="B45" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
-        <v>44</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.0)</f>
+        <v>46</v>
       </c>
       <c r="C45" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Future Perfect")</f>
@@ -2473,12 +2473,12 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Нулевой тип условных предложений")</f>
-        <v>Нулевой тип условных предложений</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Второй тип условных предложений")</f>
+        <v>Второй тип условных предложений</v>
       </c>
       <c r="B46" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45.0)</f>
-        <v>45</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),47.0)</f>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Future Perfect")</f>
@@ -2519,12 +2519,12 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Первый тип условных предложений")</f>
-        <v>Первый тип условных предложений</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Третий тип условных предложений")</f>
+        <v>Третий тип условных предложений</v>
       </c>
       <c r="B47" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.0)</f>
-        <v>46</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),48.0)</f>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Future Perfect")</f>
@@ -2565,12 +2565,12 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Второй тип условных предложений")</f>
-        <v>Второй тип условных предложений</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция «I wish..»")</f>
+        <v>Конструкция «I wish..»</v>
       </c>
       <c r="B48" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),47.0)</f>
-        <v>47</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),49.0)</f>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Present Perfect Continuous")</f>
@@ -2611,12 +2611,12 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Третий тип условных предложений")</f>
-        <v>Третий тип условных предложений</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""can""")</f>
+        <v>Модальный глагол "can"</v>
       </c>
       <c r="B49" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),48.0)</f>
-        <v>48</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.0)</f>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Present Perfect Continuous")</f>
@@ -2657,12 +2657,12 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция «I wish..»")</f>
-        <v>Конструкция «I wish..»</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""may""")</f>
+        <v>Модальный глагол "may"</v>
       </c>
       <c r="B50" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),49.0)</f>
-        <v>49</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),51.0)</f>
+        <v>51</v>
       </c>
       <c r="C50" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Present Perfect Continuous")</f>
@@ -2703,12 +2703,12 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""can""")</f>
-        <v>Модальный глагол "can"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глаголы ""shall"" и ""should""")</f>
+        <v>Модальный глаголы "shall" и "should"</v>
       </c>
       <c r="B51" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.0)</f>
-        <v>50</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.0)</f>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Present Perfect Continuous")</f>
@@ -2749,12 +2749,12 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""may""")</f>
-        <v>Модальный глагол "may"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""ought to""")</f>
+        <v>Модальный глагол "ought to"</v>
       </c>
       <c r="B52" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),51.0)</f>
-        <v>51</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),53.0)</f>
+        <v>53</v>
       </c>
       <c r="C52" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Past Perfect Continuous")</f>
@@ -2795,12 +2795,12 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глаголы ""shall"" и ""should""")</f>
-        <v>Модальный глаголы "shall" и "should"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""must""")</f>
+        <v>Модальный глагол "must"</v>
       </c>
       <c r="B53" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.0)</f>
-        <v>52</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.0)</f>
+        <v>54</v>
       </c>
       <c r="C53" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательные предложения в Past Perfect Continuous")</f>
@@ -2841,12 +2841,12 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""ought to""")</f>
-        <v>Модальный глагол "ought to"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""have to""")</f>
+        <v>Модальный глагол "have to"</v>
       </c>
       <c r="B54" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),53.0)</f>
-        <v>53</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),55.0)</f>
+        <v>55</v>
       </c>
       <c r="C54" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE""")," Вопросительные предложения в Past Perfect Continuous")</f>
@@ -2887,12 +2887,12 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""must""")</f>
-        <v>Модальный глагол "must"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""might""")</f>
+        <v>Модальный глагол "might"</v>
       </c>
       <c r="B55" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.0)</f>
-        <v>54</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.0)</f>
+        <v>56</v>
       </c>
       <c r="C55" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Past Perfect Continuous")</f>
@@ -2933,12 +2933,12 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""have to""")</f>
-        <v>Модальный глагол "have to"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Глагол be to")</f>
+        <v>Глагол be to</v>
       </c>
       <c r="B56" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),55.0)</f>
-        <v>55</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),57.0)</f>
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Present Continuous для выражения будущего")</f>
@@ -2979,12 +2979,12 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол ""might""")</f>
-        <v>Модальный глагол "might"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция used to")</f>
+        <v>Конструкция used to</v>
       </c>
       <c r="B57" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.0)</f>
-        <v>56</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58.0)</f>
+        <v>58</v>
       </c>
       <c r="C57" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Future in the Past")</f>
@@ -3025,12 +3025,12 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Глагол be to")</f>
-        <v>Глагол be to</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция to be used to")</f>
+        <v>Конструкция to be used to</v>
       </c>
       <c r="B58" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),57.0)</f>
-        <v>57</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),59.0)</f>
+        <v>59</v>
       </c>
       <c r="C58" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Вопросительные предложения в Future Perfect Continuous")</f>
@@ -3071,12 +3071,12 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция used to")</f>
-        <v>Конструкция used to</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция to be going to")</f>
+        <v>Конструкция to be going to</v>
       </c>
       <c r="B59" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58.0)</f>
-        <v>58</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),60.0)</f>
+        <v>60</v>
       </c>
       <c r="C59" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительные предложения в Future Perfect Continuous")</f>
@@ -3117,12 +3117,12 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция to be used to")</f>
-        <v>Конструкция to be used to</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Вопросительное предложение с модальным глаголом")</f>
+        <v>Вопросительное предложение с модальным глаголом</v>
       </c>
       <c r="B60" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),59.0)</f>
-        <v>59</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),61.0)</f>
+        <v>61</v>
       </c>
       <c r="C60" s="1" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Слова-маркеры Future Perfect Continuous")</f>
@@ -3163,12 +3163,12 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция to be going to")</f>
-        <v>Конструкция to be going to</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательное предложение с модальным глаголом")</f>
+        <v>Отрицательное предложение с модальным глаголом</v>
       </c>
       <c r="B61" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),60.0)</f>
-        <v>60</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),62.0)</f>
+        <v>62</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -3203,12 +3203,12 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Вопросительное предложение с модальным глаголом")</f>
-        <v>Вопросительное предложение с модальным глаголом</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительное предложение с модальным глаголом")</f>
+        <v>Утвердительное предложение с модальным глаголом</v>
       </c>
       <c r="B62" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),61.0)</f>
-        <v>61</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),63.0)</f>
+        <v>63</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -3243,12 +3243,12 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Отрицательное предложение с модальным глаголом")</f>
-        <v>Отрицательное предложение с модальным глаголом</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция Have something done")</f>
+        <v>Конструкция Have something done</v>
       </c>
       <c r="B63" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),62.0)</f>
-        <v>62</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),64.0)</f>
+        <v>64</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3283,12 +3283,12 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Утвердительное предложение с модальным глаголом")</f>
-        <v>Утвердительное предложение с модальным глаголом</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Глагол Would")</f>
+        <v>Глагол Would</v>
       </c>
       <c r="B64" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),63.0)</f>
-        <v>63</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
+        <v>65</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -3323,12 +3323,12 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция Have something done")</f>
-        <v>Конструкция Have something done</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция Had better")</f>
+        <v>Конструкция Had better</v>
       </c>
       <c r="B65" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),64.0)</f>
-        <v>64</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),67.0)</f>
+        <v>67</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -3363,12 +3363,12 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Глагол Would")</f>
-        <v>Глагол Would</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкции would prefer и would rather")</f>
+        <v>Конструкции would prefer и would rather</v>
       </c>
       <c r="B66" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
-        <v>65</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),68.0)</f>
+        <v>68</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3402,14 +3402,8 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкции had better… / would rather")</f>
-        <v>Конструкции had better… / would rather</v>
-      </c>
-      <c r="B67" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),66.0)</f>
-        <v>66</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="str">
@@ -3443,12 +3437,12 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция Had better")</f>
-        <v>Конструкция Had better</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Сложное дополнение")</f>
+        <v>Сложное дополнение</v>
       </c>
       <c r="B68" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),67.0)</f>
-        <v>67</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),70.0)</f>
+        <v>70</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -3483,12 +3477,12 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкции would prefer и would rather")</f>
-        <v>Конструкции would prefer и would rather</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Сложное подлежащее")</f>
+        <v>Сложное подлежащее</v>
       </c>
       <c r="B69" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),68.0)</f>
-        <v>68</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
+        <v>71</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3523,12 +3517,12 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Согласование времен")</f>
-        <v>Согласование времен</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол could")</f>
+        <v>Модальный глагол could</v>
       </c>
       <c r="B70" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69.0)</f>
-        <v>69</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),72.0)</f>
+        <v>72</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3563,12 +3557,12 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Сложное дополнение")</f>
-        <v>Сложное дополнение</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tag questions")</f>
+        <v>Tag questions</v>
       </c>
       <c r="B71" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),70.0)</f>
-        <v>70</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),73.0)</f>
+        <v>73</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3603,12 +3597,12 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Сложное подлежащее")</f>
-        <v>Сложное подлежащее</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Предложение с начальным it")</f>
+        <v>Предложение с начальным it</v>
       </c>
       <c r="B72" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
-        <v>71</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.0)</f>
+        <v>74</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3643,12 +3637,12 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Модальный глагол could")</f>
-        <v>Модальный глагол could</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Устойчивые сочетания прилагательных с предлогами")</f>
+        <v>Устойчивые сочетания прилагательных с предлогами</v>
       </c>
       <c r="B73" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),72.0)</f>
-        <v>72</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),75.0)</f>
+        <v>75</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3683,12 +3677,12 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tag questions")</f>
-        <v>Tag questions</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Простые предложения")</f>
+        <v>Простые предложения</v>
       </c>
       <c r="B74" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),73.0)</f>
-        <v>73</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),76.0)</f>
+        <v>76</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3723,12 +3717,12 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Предложение с начальным it")</f>
-        <v>Предложение с начальным it</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инфинитив в предложении")</f>
+        <v>Инфинитив в предложении</v>
       </c>
       <c r="B75" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.0)</f>
-        <v>74</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),78.0)</f>
+        <v>78</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3763,12 +3757,12 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Устойчивые сочетания прилагательных с предлогами")</f>
-        <v>Устойчивые сочетания прилагательных с предлогами</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция ""it+to be""")</f>
+        <v>Конструкция "it+to be"</v>
       </c>
       <c r="B76" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),75.0)</f>
-        <v>75</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
+        <v>79</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3803,12 +3797,12 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Простые предложения")</f>
-        <v>Простые предложения</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция ""it takes""")</f>
+        <v>Конструкция "it takes"</v>
       </c>
       <c r="B77" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),76.0)</f>
-        <v>76</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),80.0)</f>
+        <v>80</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3843,12 +3837,12 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Герундий в предложении")</f>
-        <v>Герундий в предложении</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительно степени прилагательного с помощью much")</f>
+        <v>Образование сравнительно степени прилагательного с помощью much</v>
       </c>
       <c r="B78" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),77.0)</f>
-        <v>77</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),81.0)</f>
+        <v>81</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3883,12 +3877,12 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инфинитив в предложении")</f>
-        <v>Инфинитив в предложении</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательного с усилением с помощью much more")</f>
+        <v>Образование сравнительной степени прилагательного с усилением с помощью much more</v>
       </c>
       <c r="B79" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),78.0)</f>
-        <v>78</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),82.0)</f>
+        <v>82</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3923,12 +3917,12 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция ""it+to be""")</f>
-        <v>Конструкция "it+to be"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательного с усилением с помощью far more")</f>
+        <v>Образование сравнительной степени прилагательного с усилением с помощью far more</v>
       </c>
       <c r="B80" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
-        <v>79</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.0)</f>
+        <v>83</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3963,12 +3957,12 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция ""it takes""")</f>
-        <v>Конструкция "it takes"</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Participle 2")</f>
+        <v>Participle 2</v>
       </c>
       <c r="B81" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),80.0)</f>
-        <v>80</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),84.0)</f>
+        <v>84</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -4003,12 +3997,12 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительно степени прилагательного с помощью much")</f>
-        <v>Образование сравнительно степени прилагательного с помощью much</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречий, совпадающих по форме с прилагательными")</f>
+        <v>Образование степеней сравнения наречий, совпадающих по форме с прилагательными</v>
       </c>
       <c r="B82" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),81.0)</f>
-        <v>81</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),85.0)</f>
+        <v>85</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -4043,12 +4037,12 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательного с усилением с помощью much more")</f>
-        <v>Образование сравнительной степени прилагательного с усилением с помощью much more</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречий, образованных от прилагательных с помощью -ly")</f>
+        <v>Образование степеней сравнения наречий, образованных от прилагательных с помощью -ly</v>
       </c>
       <c r="B83" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),82.0)</f>
-        <v>82</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),86.0)</f>
+        <v>86</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -4083,12 +4077,12 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени прилагательного с усилением с помощью far more")</f>
-        <v>Образование сравнительной степени прилагательного с усилением с помощью far more</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения многосложных наречий")</f>
+        <v>Образование степеней сравнения многосложных наречий</v>
       </c>
       <c r="B84" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.0)</f>
-        <v>83</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),87.0)</f>
+        <v>87</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -4123,12 +4117,12 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Причастие Participle 2")</f>
-        <v>Причастие Participle 2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречия: исключения")</f>
+        <v>Образование степеней сравнения наречия: исключения</v>
       </c>
       <c r="B85" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),84.0)</f>
-        <v>84</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),88.0)</f>
+        <v>88</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -4163,12 +4157,12 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречий, совпадающих по форме с прилагательными")</f>
-        <v>Образование степеней сравнения наречий, совпадающих по форме с прилагательными</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Предложения с конструкциями either ... or; neither ... nor")</f>
+        <v>Предложения с конструкциями either ... or; neither ... nor</v>
       </c>
       <c r="B86" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),85.0)</f>
-        <v>85</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),89.0)</f>
+        <v>89</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -4203,12 +4197,12 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречий, образованных от прилагательных с помощью -ly")</f>
-        <v>Образование степеней сравнения наречий, образованных от прилагательных с помощью -ly</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция be able to")</f>
+        <v>Конструкция be able to</v>
       </c>
       <c r="B87" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),86.0)</f>
-        <v>86</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),126.0)</f>
+        <v>126</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -4243,12 +4237,12 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения многосложных наречий")</f>
-        <v>Образование степеней сравнения многосложных наречий</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени наречий")</f>
+        <v>Образование сравнительной степени наречий</v>
       </c>
       <c r="B88" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),87.0)</f>
-        <v>87</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),90.0)</f>
+        <v>90</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -4283,12 +4277,12 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование степеней сравнения наречия: исключения")</f>
-        <v>Образование степеней сравнения наречия: исключения</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование превосходной степени наречий")</f>
+        <v>Образование превосходной степени наречий</v>
       </c>
       <c r="B89" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),88.0)</f>
-        <v>88</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),91.0)</f>
+        <v>91</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -4323,12 +4317,12 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Предложения с конструкциями either ... or; neither ... nor")</f>
-        <v>Предложения с конструкциями either ... or; neither ... nor</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Исключения в сравнении наречий")</f>
+        <v>Исключения в сравнении наречий</v>
       </c>
       <c r="B90" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),89.0)</f>
-        <v>89</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),92.0)</f>
+        <v>92</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -4363,12 +4357,12 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция be able to")</f>
-        <v>Конструкция be able to</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление артикля a/an перед гласными/согласными")</f>
+        <v>Употребление артикля a/an перед гласными/согласными</v>
       </c>
       <c r="B91" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),126.0)</f>
-        <v>126</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),93.0)</f>
+        <v>93</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -4403,12 +4397,12 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование сравнительной степени наречий")</f>
-        <v>Образование сравнительной степени наречий</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"For-to construction, Causative form")</f>
+        <v>For-to construction, Causative form</v>
       </c>
       <c r="B92" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),90.0)</f>
-        <v>90</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),94.0)</f>
+        <v>94</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -4443,12 +4437,12 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Образование превосходной степени наречий")</f>
-        <v>Образование превосходной степени наречий</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Относительные местоимения")</f>
+        <v>Относительные местоимения</v>
       </c>
       <c r="B93" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),91.0)</f>
-        <v>91</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),95.0)</f>
+        <v>95</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -4483,12 +4477,12 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Исключения в сравнении наречий")</f>
-        <v>Исключения в сравнении наречий</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Разница like/as")</f>
+        <v>Разница like/as</v>
       </c>
       <c r="B94" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),92.0)</f>
-        <v>92</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),97.0)</f>
+        <v>97</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4523,12 +4517,12 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление артикля a/an перед гласными/согласными")</f>
-        <v>Употребление артикля a/an перед гласными/согласными</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Собирательные существительные")</f>
+        <v>Собирательные существительные</v>
       </c>
       <c r="B95" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),93.0)</f>
-        <v>93</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),98.0)</f>
+        <v>98</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -4563,12 +4557,12 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"For-to construction, Causative form")</f>
-        <v>For-to construction, Causative form</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция For-to-Infinitive")</f>
+        <v>Конструкция For-to-Infinitive</v>
       </c>
       <c r="B96" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),94.0)</f>
-        <v>94</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),99.0)</f>
+        <v>99</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -4603,12 +4597,12 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Относительные местоимения")</f>
-        <v>Относительные местоимения</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инверсия")</f>
+        <v>Инверсия</v>
       </c>
       <c r="B97" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),95.0)</f>
-        <v>95</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),701.0)</f>
+        <v>701</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -4643,12 +4637,12 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Порядок прилагательных")</f>
-        <v>Порядок прилагательных</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Члены предложения в английском языке")</f>
+        <v>Члены предложения в английском языке</v>
       </c>
       <c r="B98" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),96.0)</f>
-        <v>96</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),702.0)</f>
+        <v>702</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -4683,12 +4677,12 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Разница like/as")</f>
-        <v>Разница like/as</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Употребление артикля an")</f>
+        <v>Употребление артикля an</v>
       </c>
       <c r="B99" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),97.0)</f>
-        <v>97</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),703.0)</f>
+        <v>703</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -4723,12 +4717,12 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Собирательные существительные")</f>
-        <v>Собирательные существительные</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Герундий в предложении")</f>
+        <v>Герундий в предложении</v>
       </c>
       <c r="B100" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),98.0)</f>
-        <v>98</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),704.0)</f>
+        <v>704</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -4763,12 +4757,12 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Конструкция For-to-Infinitive")</f>
-        <v>Конструкция For-to-Infinitive</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Participle 1 ")</f>
+        <v>Participle 1 </v>
       </c>
       <c r="B101" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),99.0)</f>
-        <v>99</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),705.0)</f>
+        <v>705</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -4803,12 +4797,12 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Инверсия")</f>
-        <v>Инверсия</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Пунктуация в сложносочиненных предложениях")</f>
+        <v>Пунктуация в сложносочиненных предложениях</v>
       </c>
       <c r="B102" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),701.0)</f>
-        <v>701</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),706.0)</f>
+        <v>706</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -4842,14 +4836,8 @@
       <c r="Z102" s="1"/>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Члены предложения в английском языке")</f>
-        <v>Члены предложения в английском языке</v>
-      </c>
-      <c r="B103" s="1">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),702.0)</f>
-        <v>702</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="str">

</xml_diff>